<commit_message>
Huge overhaul. Changed from windows to 'frames'. Use pack() and forget() to change 'frames'. Renamed several variables, moved several variables to the App class. Added a template service. Automatically saves last serached template. Removed old Search class and SearchWindow class. Moved dataclasses to the classes folder. This commit message is way too long
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Yr.</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Hometown/Previous School</t>
+          <t>Ht.</t>
         </is>
       </c>
     </row>
@@ -488,12 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Rocklin, Calif. / Whitney HS</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -520,12 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>So.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clayton, Calif. / Clayton Valley Charter</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -552,12 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Burlington, Ontario / Hutchinson CC (Kan.)</t>
+          <t>5-9</t>
         </is>
       </c>
     </row>
@@ -584,12 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Antioch, Calif. / Clayton Valley HS</t>
+          <t>6-0</t>
         </is>
       </c>
     </row>
@@ -616,12 +591,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>West Sacramento, Calif. / Granite Bay HS</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -648,12 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>So.</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Medford, Ore. / South Medford HS</t>
+          <t>6-0</t>
         </is>
       </c>
     </row>
@@ -680,12 +645,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R-So.</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Rocklin, Calif. / Granite Bay HS</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -712,12 +672,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Sacramento, Calif. / Rio Americano HS</t>
+          <t>6-4</t>
         </is>
       </c>
     </row>
@@ -744,12 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>R-Jr.</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Sacramento, Calif. / Sacramento City College</t>
+          <t>6-0</t>
         </is>
       </c>
     </row>
@@ -776,12 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Grants Pass, Ore. / Grants Pass HS</t>
+          <t>6-4</t>
         </is>
       </c>
     </row>
@@ -808,12 +753,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Sr.</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Glendora, Calif. / Long Beach State</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -840,12 +780,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>R-Fr.</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Berkeley, Calif. / Berkeley HS</t>
+          <t>6-4</t>
         </is>
       </c>
     </row>
@@ -872,12 +807,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Sr.</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Santa Cruz, Calif. / Cabrillo College</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -904,12 +834,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>R-So.</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Manila, Philippines / Cloud County CC (Kan.)</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -936,12 +861,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>So.</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Folsom, Calif. / Folsom HS</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -968,12 +888,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Concord, Calif. /</t>
+          <t>6-4</t>
         </is>
       </c>
     </row>
@@ -1000,12 +915,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Sr.</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Liberty Lake, Wash. / Spokane Falls CC</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -1032,12 +942,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Tucson, Ariz. / Sunnyside HS</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -1064,12 +969,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Las Vegas, Nev. / Faith Lutheran HS</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -1096,12 +996,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Colusa, Calif. / Chico State</t>
+          <t>6-3</t>
         </is>
       </c>
     </row>
@@ -1128,12 +1023,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Sr.</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Elk Grove, Calif. / Laguna Creek HS</t>
+          <t>6-3</t>
         </is>
       </c>
     </row>
@@ -1160,12 +1050,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Sr.</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Cameron Park, Calif. / Ponderosa HS</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -1192,12 +1077,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>R-Fr.</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>El Paso, Texas / Pebble Hills HS</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -1224,12 +1104,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Scottsdale, Ariz. / Odessa College</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -1256,12 +1131,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Delta, British Columbia / Cloud County CC (Kan.)</t>
+          <t>6-3</t>
         </is>
       </c>
     </row>
@@ -1288,12 +1158,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Oakland, Calif. / Campbell</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -1320,12 +1185,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Sacramento, Calif. / McClatchy HS</t>
+          <t>6-4</t>
         </is>
       </c>
     </row>
@@ -1352,12 +1212,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>So.</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Las Vegas, Nev. / Cimarron-Memorial HS</t>
+          <t>6-5</t>
         </is>
       </c>
     </row>
@@ -1384,12 +1239,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Fallon, Nev. /</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -1416,12 +1266,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Sr.</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Huntington Beach, Calif. / CSU Bakersfield</t>
+          <t>5-11</t>
         </is>
       </c>
     </row>
@@ -1448,12 +1293,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Redwood City, Calif. / Junipero Serra HS</t>
+          <t>5-9</t>
         </is>
       </c>
     </row>
@@ -1480,12 +1320,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>San Jose, Calif. / Archbishop Mitty HS</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -1512,12 +1347,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Sr.</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Elk Grove, Calif. / Franklin HS</t>
+          <t>6-0</t>
         </is>
       </c>
     </row>
@@ -1544,12 +1374,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Fr.</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Granite Bay, Calif. / Granite Bay HS</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -1576,12 +1401,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Phoenix, Ariz. / Grand Canyon</t>
+          <t>6-2</t>
         </is>
       </c>
     </row>
@@ -1608,12 +1428,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>So.</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Hayden, Idaho / Coeur d'Alene HS</t>
+          <t>6-3</t>
         </is>
       </c>
     </row>
@@ -1640,12 +1455,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Jr.</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Las Vegas, Nev. / Fullerton College</t>
+          <t>6-3</t>
         </is>
       </c>
     </row>
@@ -1672,12 +1482,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>R-Jr.</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Las Vegas, Nev. / Fullerton College</t>
+          <t>6-1</t>
         </is>
       </c>
     </row>
@@ -1704,12 +1509,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>R-So.</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Elk Grove, Calif. / Elk Grove HS</t>
+          <t>6-6</t>
         </is>
       </c>
     </row>

</xml_diff>